<commit_message>
Update 03 Enero 2021
</commit_message>
<xml_diff>
--- a/ModeloTransporte.xlsx
+++ b/ModeloTransporte.xlsx
@@ -8,64 +8,166 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l_alo\Downloads\ModeloTransporte\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B9EA19-76FC-4F60-9D59-4378F486D180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C3AAB7-EF3A-453D-B91B-DC304C25C3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{05D0FC68-4338-487E-8882-C1544631E011}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Hoja1!$G$21:$I$22</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Hoja2!$E$13:$H$15</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Hoja3!$E$14:$H$17</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Hoja4!$E$14:$H$17</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Hoja1!$G$23:$I$23</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Hoja2!$E$13:$H$15</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">Hoja3!$E$14:$H$17</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Hoja4!$E$14:$H$17</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Hoja1!$J$21:$J$22</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Hoja2!$E$16:$H$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">Hoja3!$E$18:$H$18</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">Hoja4!$E$18:$H$18</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Hoja1!$J$21:$J$22</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Hoja2!$I$13:$I$15</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">Hoja3!$I$14:$I$17</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">Hoja4!$I$14:$I$17</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Hoja1!$N$17</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Hoja2!$M$9</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Hoja3!$M$10</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Hoja4!$M$10</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Hoja1!$G$25:$I$25</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Hoja1!$L$21:$L$22</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Hoja2!$E$18:$H$18</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">Hoja3!$E$20:$H$20</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">Hoja4!$E$20:$H$20</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">Hoja1!$L$21:$L$22</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Hoja2!$K$13:$K$15</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">Hoja3!$K$14:$K$17</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">Hoja4!$K$14:$K$17</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -157,8 +259,266 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eduardo González Bernal</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{22A5352C-E0BB-4527-A578-65F87DD9C980}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Destino</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{2B69531D-3FB7-4DC3-8788-EF3A70D6142A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fuente</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{20DF456F-A99B-406D-A57D-0AFF778DC3F8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Capacidad</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+o cantidad de producción</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{C9142B49-E6DF-48AF-85FC-76A2E13F7F3D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cantidad</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+que requieren los clientes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eduardo González Bernal</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{4E6DACED-B9ED-44B4-8D46-264467300464}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Destino</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{85F2DFA5-918A-45F6-A6B9-5F38F1B4F1DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fuente</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{DCBF35FC-78E4-4DC4-B6F6-D7836F55F0FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Capacidad</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+o cantidad de producción</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{68A2948D-BB93-47A6-94F1-8811DABE711D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cantidad</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+que requieren los clientes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Eduardo González Bernal</author>
+  </authors>
+  <commentList>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{18321A67-7031-4AF8-8A11-EF18A36F8666}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Destino</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{163A4DAB-C3E3-41C9-B8DC-8D0D23DE1284}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fuente</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{BC3CADEB-7854-49F4-B173-D85330BC6644}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Capacidad</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+o cantidad de producción</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{3BC6714C-0F77-40BE-927E-AC34D9530145}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cantidad</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+que requieren los clientes</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="25">
   <si>
     <t>Demanda</t>
   </si>
@@ -218,6 +578,21 @@
   </si>
   <si>
     <t>RESTRICCIONES</t>
+  </si>
+  <si>
+    <t>Unidades Requeridas</t>
+  </si>
+  <si>
+    <t>Unidades Disponibles</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
   </si>
 </sst>
 </file>
@@ -323,7 +698,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -421,11 +796,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -459,6 +845,31 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -471,9 +882,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -483,11 +891,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,7 +952,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10810874" cy="1524000"/>
+          <a:ext cx="10506074" cy="1524000"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="8823370" cy="1524000"/>
         </a:xfrm>
@@ -720,7 +1131,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -757,8 +1168,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="4762500"/>
-          <a:ext cx="3048000" cy="1905000"/>
+          <a:off x="0" y="4572000"/>
+          <a:ext cx="3048000" cy="2095500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -927,6 +1338,195 @@
         <a:xfrm>
           <a:off x="3609975" y="4181475"/>
           <a:ext cx="114300" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>5291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>682625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Abrir llave 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{984A4F00-5081-46AA-9134-4ADE647FFAD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2085975" y="2862791"/>
+          <a:ext cx="120650" cy="556683"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>5291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>682625</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Abrir llave 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D57B764E-B1A0-4FB7-B809-A3C6F34ACB1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2085975" y="2862791"/>
+          <a:ext cx="120650" cy="556683"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-MX" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>5291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>682625</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Abrir llave 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5215F94F-7910-4848-8E63-C7E8D2E7A396}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2085975" y="3243791"/>
+          <a:ext cx="120650" cy="556683"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst/>
@@ -1257,24 +1857,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E34AF27-CFAF-4009-9ACC-034E91B8CFC6}">
-  <dimension ref="D11:N25"/>
+  <dimension ref="D11:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="11" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F12" s="4" t="s">
@@ -1292,10 +1893,10 @@
       <c r="J12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="19"/>
+      <c r="M12" s="23"/>
       <c r="N12" s="2">
         <f>SUM(J13:J14)</f>
         <v>280000</v>
@@ -1317,10 +1918,10 @@
       <c r="J13" s="8">
         <v>160000</v>
       </c>
-      <c r="L13" s="19" t="s">
+      <c r="L13" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="19"/>
+      <c r="M13" s="23"/>
       <c r="N13" s="2">
         <f>SUM(G15:I15)</f>
         <v>240000</v>
@@ -1342,10 +1943,10 @@
       <c r="J14" s="8">
         <v>120000</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="19"/>
+      <c r="M14" s="23"/>
       <c r="N14" s="10">
         <f>N12-N13</f>
         <v>40000</v>
@@ -1366,41 +1967,41 @@
       </c>
     </row>
     <row r="16" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="L16" s="16" t="s">
+      <c r="L16" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="17"/>
-      <c r="N16" s="18"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="15"/>
+      <c r="M17" s="24"/>
       <c r="N17" s="13">
         <f>SUMPRODUCT(G13:I14,G21:I22)</f>
         <v>940000</v>
       </c>
     </row>
     <row r="18" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
     </row>
     <row r="19" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="21" t="s">
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F20" s="4" t="s">
@@ -1448,6 +2049,9 @@
       <c r="L21" s="8">
         <v>160000</v>
       </c>
+      <c r="M21" s="19" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F22" s="11" t="s">
@@ -1472,6 +2076,7 @@
       <c r="L22" s="8">
         <v>120000</v>
       </c>
+      <c r="M22" s="19"/>
     </row>
     <row r="23" spans="4:14" x14ac:dyDescent="0.25">
       <c r="F23" s="5" t="s">
@@ -1492,10 +2097,10 @@
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="6" t="s">
         <v>7</v>
       </c>
@@ -1523,8 +2128,17 @@
         <v>90000</v>
       </c>
     </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G26" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="M21:M22"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="L12:M12"/>
@@ -1540,4 +2154,1259 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19F93BF0-371E-4510-97EA-39EAB0A4ABAA}">
+  <dimension ref="B2:M19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="23"/>
+      <c r="M3" s="2">
+        <f>SUM(I4:I6)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9">
+        <v>464</v>
+      </c>
+      <c r="F4" s="9">
+        <v>513</v>
+      </c>
+      <c r="G4" s="9">
+        <v>654</v>
+      </c>
+      <c r="H4" s="9">
+        <v>867</v>
+      </c>
+      <c r="I4" s="8">
+        <v>75</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="23"/>
+      <c r="M4" s="2">
+        <f>SUM(E7:H7)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="9">
+        <v>352</v>
+      </c>
+      <c r="F5" s="9">
+        <v>416</v>
+      </c>
+      <c r="G5" s="9">
+        <v>690</v>
+      </c>
+      <c r="H5" s="9">
+        <v>791</v>
+      </c>
+      <c r="I5" s="8">
+        <v>125</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="10">
+        <f>M3-M4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9">
+        <v>995</v>
+      </c>
+      <c r="F6" s="9">
+        <v>682</v>
+      </c>
+      <c r="G6" s="9">
+        <v>388</v>
+      </c>
+      <c r="H6" s="9">
+        <v>685</v>
+      </c>
+      <c r="I6" s="8">
+        <v>100</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>80</v>
+      </c>
+      <c r="F7" s="8">
+        <v>65</v>
+      </c>
+      <c r="G7" s="8">
+        <v>70</v>
+      </c>
+      <c r="H7" s="8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="K8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="26"/>
+      <c r="M8" s="27"/>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="13">
+        <f>SUMPRODUCT(E4:H6,E13:H15)</f>
+        <v>152535</v>
+      </c>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D10" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="16"/>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E11" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D12" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9">
+        <v>20</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>55</v>
+      </c>
+      <c r="I13" s="3">
+        <f>SUM(E13:H13)</f>
+        <v>75</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="8">
+        <v>75</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="9">
+        <v>80</v>
+      </c>
+      <c r="F14" s="9">
+        <v>45</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <f>SUM(E14:H14)</f>
+        <v>125</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="8">
+        <v>125</v>
+      </c>
+      <c r="L14" s="19"/>
+    </row>
+    <row r="15" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="9">
+        <v>0</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>70</v>
+      </c>
+      <c r="H15" s="9">
+        <v>30</v>
+      </c>
+      <c r="I15" s="3">
+        <f>SUM(E15:H15)</f>
+        <v>100</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="8">
+        <v>100</v>
+      </c>
+      <c r="L15" s="19"/>
+    </row>
+    <row r="16" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3">
+        <f>SUM(E13:E15)</f>
+        <v>80</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" ref="F16:H16" si="0">SUM(F13:F15)</f>
+        <v>65</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8">
+        <v>80</v>
+      </c>
+      <c r="F18" s="8">
+        <v>65</v>
+      </c>
+      <c r="G18" s="8">
+        <v>70</v>
+      </c>
+      <c r="H18" s="8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="L13:L15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B4370A-2D90-4B6B-8879-67449FD12563}">
+  <dimension ref="B2:M21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="23"/>
+      <c r="M3" s="2">
+        <f>SUM(I4:I7)</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9">
+        <v>3</v>
+      </c>
+      <c r="I4" s="8">
+        <v>80</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="23"/>
+      <c r="M4" s="2">
+        <f>SUM(E8:H8)</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>6</v>
+      </c>
+      <c r="G5" s="9">
+        <v>6</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8">
+        <v>30</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="10">
+        <f>M3-M4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9">
+        <v>6</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9">
+        <v>4</v>
+      </c>
+      <c r="I6" s="8">
+        <v>60</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="9">
+        <v>4</v>
+      </c>
+      <c r="F7" s="9">
+        <v>3</v>
+      </c>
+      <c r="G7" s="9">
+        <v>6</v>
+      </c>
+      <c r="H7" s="9">
+        <v>6</v>
+      </c>
+      <c r="I7" s="8">
+        <v>45</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>70</v>
+      </c>
+      <c r="F8" s="8">
+        <v>40</v>
+      </c>
+      <c r="G8" s="8">
+        <v>70</v>
+      </c>
+      <c r="H8" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="13">
+        <f>SUMPRODUCT(E4:H7,E14:H17)</f>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D11" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E12" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+    </row>
+    <row r="13" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D13" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="4:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="9">
+        <v>5</v>
+      </c>
+      <c r="F14" s="9">
+        <v>40</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
+        <v>35</v>
+      </c>
+      <c r="I14" s="3">
+        <f>SUM(E14:H14)</f>
+        <v>80</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="8">
+        <v>80</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="9">
+        <v>30</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <f>SUM(E15:H15)</f>
+        <v>30</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="8">
+        <v>30</v>
+      </c>
+      <c r="L15" s="19"/>
+    </row>
+    <row r="16" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
+        <v>60</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <f>SUM(E16:H16)</f>
+        <v>60</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="8">
+        <v>60</v>
+      </c>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="9">
+        <v>35</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>10</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <f>SUM(E17:H17)</f>
+        <v>45</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="8">
+        <v>45</v>
+      </c>
+      <c r="L17" s="19"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3">
+        <f>SUM(E14:E17)</f>
+        <v>70</v>
+      </c>
+      <c r="F18" s="3">
+        <f>SUM(F14:F17)</f>
+        <v>40</v>
+      </c>
+      <c r="G18" s="3">
+        <f>SUM(G14:G17)</f>
+        <v>70</v>
+      </c>
+      <c r="H18" s="3">
+        <f>SUM(H14:H17)</f>
+        <v>35</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
+        <v>70</v>
+      </c>
+      <c r="F20" s="8">
+        <v>40</v>
+      </c>
+      <c r="G20" s="8">
+        <v>70</v>
+      </c>
+      <c r="H20" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="E21:H21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E4E925-09F5-4F87-874A-195E407E617A}">
+  <dimension ref="B2:M21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="23"/>
+      <c r="M3" s="2">
+        <f>SUM(I4:I7)</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9">
+        <v>3</v>
+      </c>
+      <c r="I4" s="8">
+        <v>80</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="23"/>
+      <c r="M4" s="2">
+        <f>SUM(E8:H8)</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3</v>
+      </c>
+      <c r="F5" s="9">
+        <v>6</v>
+      </c>
+      <c r="G5" s="9">
+        <v>6</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8">
+        <v>30</v>
+      </c>
+      <c r="K5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="10">
+        <f>M3-M4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="9">
+        <v>6</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9">
+        <v>4</v>
+      </c>
+      <c r="I6" s="8">
+        <v>60</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="9">
+        <v>4</v>
+      </c>
+      <c r="F7" s="9">
+        <v>3</v>
+      </c>
+      <c r="G7" s="9">
+        <v>6</v>
+      </c>
+      <c r="H7" s="9">
+        <v>6</v>
+      </c>
+      <c r="I7" s="8">
+        <v>45</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>70</v>
+      </c>
+      <c r="F8" s="8">
+        <v>40</v>
+      </c>
+      <c r="G8" s="8">
+        <v>70</v>
+      </c>
+      <c r="H8" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="26"/>
+      <c r="M9" s="27"/>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="24"/>
+      <c r="M10" s="13">
+        <f>SUMPRODUCT(E4:H7,E14:H17)</f>
+        <v>620</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D11" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E12" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+    </row>
+    <row r="13" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D13" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
+        <v>40</v>
+      </c>
+      <c r="G14" s="9">
+        <v>5</v>
+      </c>
+      <c r="H14" s="9">
+        <v>35</v>
+      </c>
+      <c r="I14" s="3">
+        <f>SUM(E14:H14)</f>
+        <v>80</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="8">
+        <v>80</v>
+      </c>
+      <c r="L14" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="9">
+        <v>30</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0</v>
+      </c>
+      <c r="G15" s="9">
+        <v>0</v>
+      </c>
+      <c r="H15" s="9">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <f>SUM(E15:H15)</f>
+        <v>30</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="8">
+        <v>30</v>
+      </c>
+      <c r="L15" s="19"/>
+    </row>
+    <row r="16" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0</v>
+      </c>
+      <c r="G16" s="9">
+        <v>60</v>
+      </c>
+      <c r="H16" s="9">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <f>SUM(E16:H16)</f>
+        <v>60</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="8">
+        <v>60</v>
+      </c>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="9">
+        <v>40</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0</v>
+      </c>
+      <c r="G17" s="9">
+        <v>5</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <f>SUM(E17:H17)</f>
+        <v>45</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="8">
+        <v>45</v>
+      </c>
+      <c r="L17" s="19"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3">
+        <f>SUM(E14:E17)</f>
+        <v>70</v>
+      </c>
+      <c r="F18" s="3">
+        <f>SUM(F14:F17)</f>
+        <v>40</v>
+      </c>
+      <c r="G18" s="3">
+        <f>SUM(G14:G17)</f>
+        <v>70</v>
+      </c>
+      <c r="H18" s="3">
+        <f>SUM(H14:H17)</f>
+        <v>35</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
+        <v>70</v>
+      </c>
+      <c r="F20" s="8">
+        <v>40</v>
+      </c>
+      <c r="G20" s="8">
+        <v>70</v>
+      </c>
+      <c r="H20" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="L14:L17"/>
+    <mergeCell ref="B19:C19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>